<commit_message>
add box plots to analysis excels
</commit_message>
<xml_diff>
--- a/knn_results/results_hypo.xlsx
+++ b/knn_results/results_hypo.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tair\PycharmProjects\MAI-IML-W3\knn_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B4356FC-62F8-44D7-B6EF-8614AEA5EF0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28DCDC1-B91B-47C3-8541-0D6F7051184A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hypo_results" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,73 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">hypo_results!$A$1:$F$109</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">metric!$A$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">metric!$A$1:$A$37</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">metric!$B$2:$B$37</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">metric!$C$1</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">metric!$C$2:$C$37</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">metric!$A$1</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">metric!$A$2:$A$37</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">metric!$B$1</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">metric!$B$2:$B$37</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">metric!$C$1</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">metric!$C$2:$C$37</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">metric!$A$1</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">metric!$A$2:$A$37</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">metric!$A$2:$A$37</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">metric!$B$1</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">metric!$B$2:$B$37</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">metric!$C$1</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">metric!$C$2:$C$37</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">metric!$A$1</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">metric!$A$2:$A$37</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">metric!$B$1</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">metric!$B$2:$B$37</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">metric!$C$1</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">metric!$B$1</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">metric!$C$2:$C$37</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">k!$A$1</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">k!$A$2:$A$28</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">k!$B$1</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">k!$B$2:$B$28</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">k!$C$1</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">k!$C$2:$C$28</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">k!$D$1</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">k!$D$2:$D$28</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">k!$A$2:$A$28</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">metric!$B$2:$B$37</definedName>
+    <definedName name="_xlchart.v1.40" hidden="1">k!$B$2:$B$28</definedName>
+    <definedName name="_xlchart.v1.41" hidden="1">k!$C$2:$C$28</definedName>
+    <definedName name="_xlchart.v1.42" hidden="1">k!$D$2:$D$28</definedName>
+    <definedName name="_xlchart.v1.43" hidden="1">voting!$A$1</definedName>
+    <definedName name="_xlchart.v1.44" hidden="1">voting!$A$2:$A$37</definedName>
+    <definedName name="_xlchart.v1.45" hidden="1">voting!$B$1</definedName>
+    <definedName name="_xlchart.v1.46" hidden="1">voting!$B$2:$B$37</definedName>
+    <definedName name="_xlchart.v1.47" hidden="1">voting!$C$1</definedName>
+    <definedName name="_xlchart.v1.48" hidden="1">voting!$C$2:$C$37</definedName>
+    <definedName name="_xlchart.v1.49" hidden="1">voting!$A$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">metric!$C$1</definedName>
+    <definedName name="_xlchart.v1.50" hidden="1">voting!$A$2:$A$37</definedName>
+    <definedName name="_xlchart.v1.51" hidden="1">voting!$B$1</definedName>
+    <definedName name="_xlchart.v1.52" hidden="1">voting!$B$2:$B$37</definedName>
+    <definedName name="_xlchart.v1.53" hidden="1">voting!$C$1</definedName>
+    <definedName name="_xlchart.v1.54" hidden="1">voting!$C$2:$C$37</definedName>
+    <definedName name="_xlchart.v1.55" hidden="1">voting!$A$2:$A$37</definedName>
+    <definedName name="_xlchart.v1.56" hidden="1">voting!$B$2:$B$37</definedName>
+    <definedName name="_xlchart.v1.57" hidden="1">voting!$C$2:$C$37</definedName>
+    <definedName name="_xlchart.v1.58" hidden="1">weightings!$A$2:$A$37</definedName>
+    <definedName name="_xlchart.v1.59" hidden="1">weightings!$B$2:$B$37</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">metric!$C$2:$C$37</definedName>
+    <definedName name="_xlchart.v1.60" hidden="1">weightings!$C$2:$C$37</definedName>
+    <definedName name="_xlchart.v1.61" hidden="1">weightings!$A$1</definedName>
+    <definedName name="_xlchart.v1.62" hidden="1">weightings!$A$2:$A$37</definedName>
+    <definedName name="_xlchart.v1.63" hidden="1">weightings!$B$1</definedName>
+    <definedName name="_xlchart.v1.64" hidden="1">weightings!$B$2:$B$37</definedName>
+    <definedName name="_xlchart.v1.65" hidden="1">weightings!$C$1</definedName>
+    <definedName name="_xlchart.v1.66" hidden="1">weightings!$C$2:$C$37</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">metric!$A$1</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">metric!$A$2:$A$37</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">metric!$B$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -155,7 +222,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -667,7 +734,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -678,6 +745,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -734,6 +802,3699 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.8</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.10</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="2">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.12</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{60DE7476-949A-4413-AE58-AD43D751C43F}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.7</cx:f>
+              <cx:v>camberra</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{EC8C6A2C-727C-497A-BF1E-E5CD8C147C6D}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.9</cx:f>
+              <cx:v>euclidean</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{25D7C1A1-5AE0-4B01-A3A1-35DCE9338E55}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.11</cx:f>
+              <cx:v>manhattan</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="2"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0" hidden="1">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>accuracy</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>accuracy</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx2.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.20</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.22</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="2">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.24</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{F3E5E1B9-7ED5-44A6-ADF9-35935F336139}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.19</cx:f>
+              <cx:v>camberra</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{D2DA33B6-9EE5-41FE-B2E3-78D1758E1CBC}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.21</cx:f>
+              <cx:v>euclidean</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{1C41A2A0-3A94-4E7D-BECB-91178E4891F5}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.23</cx:f>
+              <cx:v>manhattan</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="2"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0" hidden="1">
+        <cx:catScaling gapWidth="1"/>
+        <cx:title/>
+        <cx:tickLabels/>
+        <cx:txPr>
+          <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:endParaRPr>
+          </a:p>
+        </cx:txPr>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:title/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx3.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.32</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.34</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="2">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.36</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="3">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.38</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{36FA7DD3-7FB8-4B93-9045-055CF9FE69BF}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.31</cx:f>
+              <cx:v>k1</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{B86CC9C0-3F84-45B9-BEE7-9A78ED3D4C57}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.33</cx:f>
+              <cx:v>k3</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{22A3921F-5CA3-42E0-91BD-D84C04ACB939}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.35</cx:f>
+              <cx:v>k5</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="2"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{2A547B62-3AB4-4A0C-B0F8-C5552CE10DC7}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.37</cx:f>
+              <cx:v>k7</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="3"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx4.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.50</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.52</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="2">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.54</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{E5352E6C-D853-4F7B-8DEB-A720291BE09E}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.49</cx:f>
+              <cx:v>inverse_distance_weighted</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{269CF19C-8742-42F8-903A-05584308982B}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.51</cx:f>
+              <cx:v>majority_class</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{815F7E96-F0D7-41C9-B5BA-64DB4751AB97}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.53</cx:f>
+              <cx:v>sheppards_work</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="2"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0" hidden="1">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>accuracy</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>accuracy</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx5.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.62</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.64</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="2">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.66</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{D117C914-79C5-4786-8876-63A08FF36768}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.61</cx:f>
+              <cx:v>equal_weight</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{0E48F266-F040-4901-99E0-3D13618DC402}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.63</cx:f>
+              <cx:v>info_gain</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{2D0E0570-6392-46DA-B80E-5F94F260EE7D}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.65</cx:f>
+              <cx:v>reliefF</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="2"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0" hidden="1">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>accuracy</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>accuracy</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>49530</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>49530</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Chart 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE13DD58-E391-4D12-9CD3-2AEEFAA5E352}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3535680" y="3006090"/>
+              <a:ext cx="4572000" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>411480</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>11430</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>510540</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>11430</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="4" name="Chart 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0727C2A4-9F59-4841-B8DA-7E5EFB808044}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3459480" y="3150870"/>
+              <a:ext cx="4572000" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>335280</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Chart 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99E6983F-5C79-4104-BCA5-472D66B51759}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3680460" y="3166110"/>
+              <a:ext cx="4572000" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>156210</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>156210</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Chart 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13478768-8FDB-4D73-8C8D-9D31111D2CB7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4259580" y="3112770"/>
+              <a:ext cx="4572000" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Chart 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80D980D8-DBE6-44E7-BDBF-92AD985560AB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3322320" y="2907030"/>
+              <a:ext cx="4792980" cy="2929890"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1032,12 +4793,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1066,7 +4826,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1086,7 +4846,7 @@
         <v>0.79002039432525595</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1106,7 +4866,7 @@
         <v>1.8223264694213801</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1126,7 +4886,7 @@
         <v>1.7087178945541299</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1146,7 +4906,7 @@
         <v>0.80222947597503602</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1166,7 +4926,7 @@
         <v>1.8271151304244899</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1246,7 +5006,7 @@
         <v>1.74384663105011</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1266,7 +5026,7 @@
         <v>0.79445757865905697</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1286,7 +5046,7 @@
         <v>1.9024913311004601</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1306,7 +5066,7 @@
         <v>1.7232429027557301</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1326,7 +5086,7 @@
         <v>0.80384376049041695</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1346,7 +5106,7 @@
         <v>1.9052603483199999</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1426,7 +5186,7 @@
         <v>1.7694867134094201</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1446,7 +5206,7 @@
         <v>0.79683787822723295</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -1466,7 +5226,7 @@
         <v>1.9430340051651001</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -1486,7 +5246,7 @@
         <v>1.7421351671218801</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -1506,7 +5266,7 @@
         <v>0.80989871025085403</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1526,7 +5286,7 @@
         <v>1.94906997680664</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -1606,7 +5366,7 @@
         <v>1.7267562389373701</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -1626,7 +5386,7 @@
         <v>0.802449607849121</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -1646,7 +5406,7 @@
         <v>1.9744885921478199</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -1666,7 +5426,7 @@
         <v>1.7173536777496301</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -1686,7 +5446,7 @@
         <v>0.80471229553222601</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -1706,7 +5466,7 @@
         <v>1.9845877647399901</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>0</v>
       </c>
@@ -1786,7 +5546,7 @@
         <v>1.7248673915863</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -1806,7 +5566,7 @@
         <v>0.79428086280822696</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -1826,7 +5586,7 @@
         <v>1.8213909626007001</v>
       </c>
     </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -1846,7 +5606,7 @@
         <v>1.70889325141906</v>
       </c>
     </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -1866,7 +5626,7 @@
         <v>0.79710698127746504</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -1886,7 +5646,7 @@
         <v>1.8149605751037501</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>7</v>
       </c>
@@ -1966,7 +5726,7 @@
         <v>1.7131762504577599</v>
       </c>
     </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>7</v>
       </c>
@@ -1986,7 +5746,7 @@
         <v>0.79711215496063204</v>
       </c>
     </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>7</v>
       </c>
@@ -2006,7 +5766,7 @@
         <v>1.8803970813751201</v>
       </c>
     </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>7</v>
       </c>
@@ -2026,7 +5786,7 @@
         <v>1.7238685846328701</v>
       </c>
     </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -2046,7 +5806,7 @@
         <v>0.80158209800720204</v>
       </c>
     </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>7</v>
       </c>
@@ -2066,7 +5826,7 @@
         <v>1.89834566116333</v>
       </c>
     </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -2146,7 +5906,7 @@
         <v>1.7306319475173899</v>
       </c>
     </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>7</v>
       </c>
@@ -2166,7 +5926,7 @@
         <v>0.79225687980651804</v>
       </c>
     </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>7</v>
       </c>
@@ -2186,7 +5946,7 @@
         <v>1.92895119190216</v>
       </c>
     </row>
-    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>7</v>
       </c>
@@ -2206,7 +5966,7 @@
         <v>1.7108053445816001</v>
       </c>
     </row>
-    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>7</v>
       </c>
@@ -2226,7 +5986,7 @@
         <v>0.80017292499542203</v>
       </c>
     </row>
-    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>7</v>
       </c>
@@ -2246,7 +6006,7 @@
         <v>1.93194470405578</v>
       </c>
     </row>
-    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>7</v>
       </c>
@@ -2326,7 +6086,7 @@
         <v>1.7153373003005901</v>
       </c>
     </row>
-    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>7</v>
       </c>
@@ -2346,7 +6106,7 @@
         <v>0.79383332729339595</v>
       </c>
     </row>
-    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>7</v>
       </c>
@@ -2366,7 +6126,7 @@
         <v>1.9910468816757201</v>
       </c>
     </row>
-    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>7</v>
       </c>
@@ -2386,7 +6146,7 @@
         <v>1.72804636955261</v>
       </c>
     </row>
-    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>7</v>
       </c>
@@ -2406,7 +6166,7 @@
         <v>0.80615425109863204</v>
       </c>
     </row>
-    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>7</v>
       </c>
@@ -2426,7 +6186,7 @@
         <v>1.9669403553008999</v>
       </c>
     </row>
-    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>7</v>
       </c>
@@ -2506,7 +6266,7 @@
         <v>1.74069526195526</v>
       </c>
     </row>
-    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>8</v>
       </c>
@@ -2526,7 +6286,7 @@
         <v>1.4619272708892801</v>
       </c>
     </row>
-    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>8</v>
       </c>
@@ -2546,7 +6306,7 @@
         <v>2.4781369209289501</v>
       </c>
     </row>
-    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>8</v>
       </c>
@@ -2566,7 +6326,7 @@
         <v>2.3648387670516899</v>
       </c>
     </row>
-    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>8</v>
       </c>
@@ -2586,7 +6346,7 @@
         <v>1.464093875885</v>
       </c>
     </row>
-    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>8</v>
       </c>
@@ -2606,7 +6366,7 @@
         <v>2.4833302497863698</v>
       </c>
     </row>
-    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>8</v>
       </c>
@@ -2686,7 +6446,7 @@
         <v>2.3826966762542701</v>
       </c>
     </row>
-    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>8</v>
       </c>
@@ -2706,7 +6466,7 @@
         <v>1.45810139179229</v>
       </c>
     </row>
-    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>8</v>
       </c>
@@ -2726,7 +6486,7 @@
         <v>2.59986093044281</v>
       </c>
     </row>
-    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>8</v>
       </c>
@@ -2746,7 +6506,7 @@
         <v>2.4209913253784099</v>
       </c>
     </row>
-    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>8</v>
       </c>
@@ -2766,7 +6526,7 @@
         <v>1.4907921552657999</v>
       </c>
     </row>
-    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>8</v>
       </c>
@@ -2786,7 +6546,7 @@
         <v>2.7058030843734699</v>
       </c>
     </row>
-    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>8</v>
       </c>
@@ -2866,7 +6626,7 @@
         <v>2.3785461664199801</v>
       </c>
     </row>
-    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>8</v>
       </c>
@@ -2886,7 +6646,7 @@
         <v>1.4632226705551099</v>
       </c>
     </row>
-    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>8</v>
       </c>
@@ -2906,7 +6666,7 @@
         <v>2.6296358585357602</v>
       </c>
     </row>
-    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>8</v>
       </c>
@@ -2926,7 +6686,7 @@
         <v>2.3965582847595202</v>
       </c>
     </row>
-    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>8</v>
       </c>
@@ -2946,7 +6706,7 @@
         <v>1.4698182344436601</v>
       </c>
     </row>
-    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>8</v>
       </c>
@@ -2966,7 +6726,7 @@
         <v>2.61098532676696</v>
       </c>
     </row>
-    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>8</v>
       </c>
@@ -3046,7 +6806,7 @@
         <v>2.3969912290573099</v>
       </c>
     </row>
-    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>8</v>
       </c>
@@ -3066,7 +6826,7 @@
         <v>1.4614236593246399</v>
       </c>
     </row>
-    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>8</v>
       </c>
@@ -3086,7 +6846,7 @@
         <v>2.6578476428985498</v>
       </c>
     </row>
-    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>8</v>
       </c>
@@ -3106,7 +6866,7 @@
         <v>2.4126720428466699</v>
       </c>
     </row>
-    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>8</v>
       </c>
@@ -3126,7 +6886,7 @@
         <v>1.47044057846069</v>
       </c>
     </row>
-    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>8</v>
       </c>
@@ -3146,7 +6906,7 @@
         <v>2.64399206638336</v>
       </c>
     </row>
-    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>8</v>
       </c>
@@ -3227,28 +6987,23 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F109">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="sheppards_work"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:F109" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection sqref="A1:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -3339,7 +7094,7 @@
         <v>0.9799688057040995</v>
       </c>
       <c r="K5" s="1">
-        <v>4.7692752356168132E-5</v>
+        <v>4.7692752356168098E-5</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -3818,18 +7573,22 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -4398,15 +8157,16 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4984,16 +8744,15 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
-    </sheetView>
+    <sheetView topLeftCell="A10" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5237,8 +8996,8 @@
       <c r="J12" s="1">
         <v>18.665300006144172</v>
       </c>
-      <c r="K12" s="1">
-        <v>1.1595206612649053E-7</v>
+      <c r="K12" s="6">
+        <v>1.15952066126491E-7</v>
       </c>
       <c r="L12" s="1">
         <v>3.0828520162818216</v>
@@ -5568,5 +9327,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>